<commit_message>
Responsividade do site institucional
</commit_message>
<xml_diff>
--- a/Documentacao/Sprint 3/Backlog/HFSystem_Backlog.xlsx
+++ b/Documentacao/Sprint 3/Backlog/HFSystem_Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e27a146a09249998/Área de Trabalho/HFSystem/Documentacao/Sprint 3/Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\1 - Documentos\2 - Acessos\Desktop\Projetos\Projetos em grupo\HFSystem\Documentacao\Sprint 3\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{81EE869E-8AC5-4976-9CDC-784C0E5D2F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F716292B-E0E2-4BBC-ADC8-03B050263D7F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4877CDA-4D07-4A38-9B37-6285C5CC872F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFSystem" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="122">
   <si>
     <t>BACKLOG</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>Integração da API de clima</t>
+  </si>
+  <si>
+    <t>EMBED</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -835,9 +838,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3399,8 +3399,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B1:U76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="48" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4687,7 +4687,7 @@
       <c r="K38" s="10"/>
     </row>
     <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.45">
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C39" s="11" t="s">
@@ -4718,7 +4718,7 @@
       <c r="K39" s="10"/>
     </row>
     <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.45">
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="11" t="s">
         <v>77</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -4749,7 +4749,7 @@
       <c r="K40" s="10"/>
     </row>
     <row r="41" spans="2:11" ht="18" x14ac:dyDescent="0.45">
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C41" s="11" t="s">
@@ -4780,7 +4780,7 @@
       <c r="K41" s="10"/>
     </row>
     <row r="42" spans="2:11" ht="18" x14ac:dyDescent="0.45">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="11" t="s">
         <v>79</v>
       </c>
       <c r="C42" s="11" t="s">
@@ -4811,7 +4811,7 @@
       <c r="K42" s="10"/>
     </row>
     <row r="43" spans="2:11" ht="18" x14ac:dyDescent="0.45">
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -4842,7 +4842,7 @@
       <c r="K43" s="10"/>
     </row>
     <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.45">
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="11" t="s">
         <v>81</v>
       </c>
       <c r="C44" s="11" t="s">
@@ -4873,7 +4873,7 @@
       <c r="K44" s="10"/>
     </row>
     <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.45">
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="11" t="s">
         <v>82</v>
       </c>
       <c r="C45" s="11" t="s">
@@ -4904,7 +4904,7 @@
       <c r="K45" s="10"/>
     </row>
     <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.45">
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -4935,7 +4935,7 @@
       <c r="K46" s="10"/>
     </row>
     <row r="47" spans="2:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="B47" s="46" t="s">
+      <c r="B47" s="11" t="s">
         <v>120</v>
       </c>
       <c r="C47" s="11" t="s">
@@ -4963,7 +4963,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55" s="16"/>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>